<commit_message>
KLRNS-0039 | Danilo Novakovic | Fixed bug where stats were not loading properly for players that already played in previous season.
</commit_message>
<xml_diff>
--- a/test-data/players-exist-from-previous-season/new_season/stats-teams-becej.xlsx
+++ b/test-data/players-exist-from-previous-season/new_season/stats-teams-becej.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\basketballleague\test-data\players-exist-from-previous-season\new_season\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B54DC7-8853-41D0-9EB2-3FE34317E7E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AEC987-E91D-425C-A762-EA6217B188E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="28575" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -792,22 +792,76 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -816,67 +870,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1220,7 +1220,7 @@
   <dimension ref="B3:Q257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="19">
-        <v>42260</v>
+        <v>42626</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -2389,19 +2389,19 @@
         <v>46</v>
       </c>
       <c r="D4" s="26"/>
-      <c r="K4" s="36">
+      <c r="K4" s="54">
         <f>GAME1!B5</f>
-        <v>42260</v>
-      </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="37" t="str">
+        <v>42626</v>
+      </c>
+      <c r="L4" s="54"/>
+      <c r="M4" s="55" t="str">
         <f xml:space="preserve"> "[vs " &amp; GAME1!B4 &amp; "]"</f>
         <v>[vs apsolventi]</v>
       </c>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
     </row>
     <row r="5" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="18"/>
@@ -2468,19 +2468,19 @@
       </c>
     </row>
     <row r="8" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30">
+      <c r="B8" s="56">
         <f>GAME1!C4</f>
         <v>4</v>
       </c>
-      <c r="C8" s="32" t="str">
+      <c r="C8" s="57" t="str">
         <f>GAME1!D4</f>
         <v>Momčilo Češljević</v>
       </c>
-      <c r="D8" s="53">
+      <c r="D8" s="31">
         <f>GAME1!E4</f>
         <v>6</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="37">
         <f>GAME1!G4*2+GAME1!I4*3+GAME1!K4+GAME1!L4+GAME1!M4+GAME1!N4+GAME1!P4+GAME1!Q4-GAME1!F4-GAME1!H4-GAME1!J4-GAME1!O4</f>
         <v>42</v>
       </c>
@@ -2496,44 +2496,44 @@
       <c r="I8" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="56">
         <f>GAME1!L4+GAME1!M4</f>
         <v>12</v>
       </c>
-      <c r="K8" s="34">
+      <c r="K8" s="58">
         <f>GAME1!L4</f>
         <v>6</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="57">
         <f>GAME1!M4</f>
         <v>6</v>
       </c>
-      <c r="M8" s="30">
+      <c r="M8" s="56">
         <f>GAME1!N4</f>
         <v>6</v>
       </c>
-      <c r="N8" s="44">
+      <c r="N8" s="33">
         <f>GAME1!O4</f>
         <v>6</v>
       </c>
-      <c r="O8" s="34">
+      <c r="O8" s="58">
         <f>GAME1!P4</f>
         <v>6</v>
       </c>
-      <c r="P8" s="34">
+      <c r="P8" s="58">
         <f>GAME1!Q4</f>
         <v>6</v>
       </c>
-      <c r="Q8" s="32">
+      <c r="Q8" s="57">
         <f>GAME1!G4*2+GAME1!I4*3+GAME1!K4</f>
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="31"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="52"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="3" t="s">
         <v>45</v>
       </c>
@@ -2546,29 +2546,29 @@
       <c r="I9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="33"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="46"/>
     </row>
     <row r="10" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="31">
+      <c r="B10" s="43">
         <f>GAME1!C5</f>
         <v>5</v>
       </c>
-      <c r="C10" s="33" t="str">
+      <c r="C10" s="46" t="str">
         <f>GAME1!D5</f>
         <v>Milan Brkljač</v>
       </c>
-      <c r="D10" s="50">
+      <c r="D10" s="36">
         <f>GAME1!E5</f>
         <v>19</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="30">
         <f>GAME1!G5*2+GAME1!I5*3+GAME1!K5+GAME1!L5+GAME1!M5+GAME1!N5+GAME1!P5+GAME1!Q5-GAME1!F5-GAME1!H5-GAME1!J5-GAME1!O5</f>
         <v>0</v>
       </c>
@@ -2587,44 +2587,44 @@
       <c r="I10" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="43">
         <f>GAME1!L5+GAME1!M5</f>
         <v>2</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K10" s="42">
         <f>GAME1!L5</f>
         <v>1</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="46">
         <f>GAME1!M5</f>
         <v>1</v>
       </c>
-      <c r="M10" s="31">
+      <c r="M10" s="43">
         <f>GAME1!N5</f>
         <v>1</v>
       </c>
-      <c r="N10" s="56">
+      <c r="N10" s="35">
         <f>GAME1!O5</f>
         <v>2</v>
       </c>
-      <c r="O10" s="35">
+      <c r="O10" s="42">
         <f>GAME1!P5</f>
         <v>0</v>
       </c>
-      <c r="P10" s="35">
+      <c r="P10" s="42">
         <f>GAME1!Q5</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="38">
+      <c r="Q10" s="40">
         <f>GAME1!G5*2+GAME1!I5*3+GAME1!K5</f>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="31"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="30"/>
       <c r="F11" s="3">
         <f>(GAME1!G5+GAME1!I5)/(GAME1!G5+GAME1!F5+GAME1!I5+GAME1!H5)</f>
         <v>0.25</v>
@@ -2640,29 +2640,29 @@
       <c r="I11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="39"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="41"/>
     </row>
     <row r="12" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="31">
+      <c r="B12" s="43">
         <f>GAME1!C6</f>
         <v>6</v>
       </c>
-      <c r="C12" s="33" t="str">
+      <c r="C12" s="46" t="str">
         <f>GAME1!D6</f>
         <v>Dejan Ćelić</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="36">
         <f>GAME1!E6</f>
         <v>17</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="30">
         <f>GAME1!G6*2+GAME1!I6*3+GAME1!K6+GAME1!L6+GAME1!M6+GAME1!N6+GAME1!P6+GAME1!Q6-GAME1!F6-GAME1!H6-GAME1!J6-GAME1!O6</f>
         <v>-1</v>
       </c>
@@ -2680,44 +2680,44 @@
       <c r="I12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="43">
         <f>GAME1!L6+GAME1!M6</f>
         <v>0</v>
       </c>
-      <c r="K12" s="35">
+      <c r="K12" s="42">
         <f>GAME1!L6</f>
         <v>0</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12" s="46">
         <f>GAME1!M6</f>
         <v>0</v>
       </c>
-      <c r="M12" s="31">
+      <c r="M12" s="43">
         <f>GAME1!N6</f>
         <v>0</v>
       </c>
-      <c r="N12" s="56">
+      <c r="N12" s="35">
         <f>GAME1!O6</f>
         <v>0</v>
       </c>
-      <c r="O12" s="35">
+      <c r="O12" s="42">
         <f>GAME1!P6</f>
         <v>0</v>
       </c>
-      <c r="P12" s="35">
+      <c r="P12" s="42">
         <f>GAME1!Q6</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="38">
+      <c r="Q12" s="40">
         <f>GAME1!G6*2+GAME1!I6*3+GAME1!K6</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="31"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="52"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="3">
         <f>(GAME1!G6+GAME1!I6)/(GAME1!G6+GAME1!F6+GAME1!I6+GAME1!H6)</f>
         <v>0</v>
@@ -2732,29 +2732,29 @@
       <c r="I13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="31"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="39"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="41"/>
     </row>
     <row r="14" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="31">
+      <c r="B14" s="43">
         <f>GAME1!C7</f>
         <v>7</v>
       </c>
-      <c r="C14" s="33" t="str">
+      <c r="C14" s="46" t="str">
         <f>GAME1!D7</f>
         <v>Dragan Gligorović</v>
       </c>
-      <c r="D14" s="50">
+      <c r="D14" s="36">
         <f>GAME1!E7</f>
         <v>8</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="30">
         <f>GAME1!G7*2+GAME1!I7*3+GAME1!K7+GAME1!L7+GAME1!M7+GAME1!N7+GAME1!P7+GAME1!Q7-GAME1!F7-GAME1!H7-GAME1!J7-GAME1!O7</f>
         <v>2</v>
       </c>
@@ -2770,44 +2770,44 @@
       <c r="I14" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="43">
         <f>GAME1!L7+GAME1!M7</f>
         <v>0</v>
       </c>
-      <c r="K14" s="35">
+      <c r="K14" s="42">
         <f>GAME1!L7</f>
         <v>0</v>
       </c>
-      <c r="L14" s="33">
+      <c r="L14" s="46">
         <f>GAME1!M7</f>
         <v>0</v>
       </c>
-      <c r="M14" s="31">
+      <c r="M14" s="43">
         <f>GAME1!N7</f>
         <v>2</v>
       </c>
-      <c r="N14" s="56">
+      <c r="N14" s="35">
         <f>GAME1!O7</f>
         <v>0</v>
       </c>
-      <c r="O14" s="35">
+      <c r="O14" s="42">
         <f>GAME1!P7</f>
         <v>0</v>
       </c>
-      <c r="P14" s="35">
+      <c r="P14" s="42">
         <f>GAME1!Q7</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="38">
+      <c r="Q14" s="40">
         <f>GAME1!G7*2+GAME1!I7*3+GAME1!K7</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="31"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="52"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="30"/>
       <c r="F15" s="3" t="s">
         <v>45</v>
       </c>
@@ -2820,29 +2820,29 @@
       <c r="I15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J15" s="31"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="39"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="41"/>
     </row>
     <row r="16" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="31">
+      <c r="B16" s="43">
         <f>GAME1!C8</f>
         <v>8</v>
       </c>
-      <c r="C16" s="33" t="str">
+      <c r="C16" s="46" t="str">
         <f>GAME1!D8</f>
         <v>Atila Horvat</v>
       </c>
-      <c r="D16" s="50">
+      <c r="D16" s="36">
         <f>GAME1!E8</f>
         <v>18</v>
       </c>
-      <c r="E16" s="52">
+      <c r="E16" s="30">
         <f>GAME1!G8*2+GAME1!I8*3+GAME1!K8+GAME1!L8+GAME1!M8+GAME1!N8+GAME1!P8+GAME1!Q8-GAME1!F8-GAME1!H8-GAME1!J8-GAME1!O8</f>
         <v>2</v>
       </c>
@@ -2860,44 +2860,44 @@
       <c r="I16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="43">
         <f>GAME1!L8+GAME1!M8</f>
         <v>2</v>
       </c>
-      <c r="K16" s="35">
+      <c r="K16" s="42">
         <f>GAME1!L8</f>
         <v>0</v>
       </c>
-      <c r="L16" s="33">
+      <c r="L16" s="46">
         <f>GAME1!M8</f>
         <v>2</v>
       </c>
-      <c r="M16" s="31">
+      <c r="M16" s="43">
         <f>GAME1!N8</f>
         <v>1</v>
       </c>
-      <c r="N16" s="56">
+      <c r="N16" s="35">
         <f>GAME1!O8</f>
         <v>0</v>
       </c>
-      <c r="O16" s="35">
+      <c r="O16" s="42">
         <f>GAME1!P8</f>
         <v>0</v>
       </c>
-      <c r="P16" s="35">
+      <c r="P16" s="42">
         <f>GAME1!Q8</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="38">
+      <c r="Q16" s="40">
         <f>GAME1!G8*2+GAME1!I8*3+GAME1!K8</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="31"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="52"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="3">
         <f>(GAME1!G8+GAME1!I8)/(GAME1!G8+GAME1!F8+GAME1!I8+GAME1!H8)</f>
         <v>0</v>
@@ -2912,29 +2912,29 @@
       <c r="I17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="31"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="39"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="41"/>
     </row>
     <row r="18" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="31">
+      <c r="B18" s="43">
         <f>GAME1!C9</f>
         <v>9</v>
       </c>
-      <c r="C18" s="33" t="str">
+      <c r="C18" s="46" t="str">
         <f>GAME1!D9</f>
         <v>Siniša Švedić</v>
       </c>
-      <c r="D18" s="50">
+      <c r="D18" s="36">
         <f>GAME1!E9</f>
         <v>14</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="30">
         <f>GAME1!G9*2+GAME1!I9*3+GAME1!K9+GAME1!L9+GAME1!M9+GAME1!N9+GAME1!P9+GAME1!Q9-GAME1!F9-GAME1!H9-GAME1!J9-GAME1!O9</f>
         <v>0</v>
       </c>
@@ -2952,44 +2952,44 @@
       <c r="I18" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="31">
+      <c r="J18" s="43">
         <f>GAME1!L9+GAME1!M9</f>
         <v>1</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="42">
         <f>GAME1!L9</f>
         <v>0</v>
       </c>
-      <c r="L18" s="33">
+      <c r="L18" s="46">
         <f>GAME1!M9</f>
         <v>1</v>
       </c>
-      <c r="M18" s="31">
+      <c r="M18" s="43">
         <f>GAME1!N9</f>
         <v>1</v>
       </c>
-      <c r="N18" s="56">
+      <c r="N18" s="35">
         <f>GAME1!O9</f>
         <v>1</v>
       </c>
-      <c r="O18" s="35">
+      <c r="O18" s="42">
         <f>GAME1!P9</f>
         <v>0</v>
       </c>
-      <c r="P18" s="35">
+      <c r="P18" s="42">
         <f>GAME1!Q9</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="38">
+      <c r="Q18" s="40">
         <f>GAME1!G9*2+GAME1!I9*3+GAME1!K9</f>
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="31"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="30"/>
       <c r="F19" s="3">
         <f>(GAME1!G9+GAME1!I9)/(GAME1!G9+GAME1!F9+GAME1!I9+GAME1!H9)</f>
         <v>0.2</v>
@@ -3004,29 +3004,29 @@
       <c r="I19" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="31"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="39"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="41"/>
     </row>
     <row r="20" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="31">
+      <c r="B20" s="43">
         <f>GAME1!C10</f>
         <v>10</v>
       </c>
-      <c r="C20" s="33" t="str">
+      <c r="C20" s="46" t="str">
         <f>GAME1!D10</f>
         <v>Vladimir Bunjevački</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20" s="36">
         <f>GAME1!E10</f>
         <v>10</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="30">
         <f>GAME1!G10*2+GAME1!I10*3+GAME1!K10+GAME1!L10+GAME1!M10+GAME1!N10+GAME1!P10+GAME1!Q10-GAME1!F10-GAME1!H10-GAME1!J10-GAME1!O10</f>
         <v>0</v>
       </c>
@@ -3042,44 +3042,44 @@
       <c r="I20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="31">
+      <c r="J20" s="43">
         <f>GAME1!L10+GAME1!M10</f>
         <v>0</v>
       </c>
-      <c r="K20" s="35">
+      <c r="K20" s="42">
         <f>GAME1!L10</f>
         <v>0</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="46">
         <f>GAME1!M10</f>
         <v>0</v>
       </c>
-      <c r="M20" s="31">
+      <c r="M20" s="43">
         <f>GAME1!N10</f>
         <v>0</v>
       </c>
-      <c r="N20" s="56">
+      <c r="N20" s="35">
         <f>GAME1!O10</f>
         <v>0</v>
       </c>
-      <c r="O20" s="35">
+      <c r="O20" s="42">
         <f>GAME1!P10</f>
         <v>0</v>
       </c>
-      <c r="P20" s="35">
+      <c r="P20" s="42">
         <f>GAME1!Q10</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="38">
+      <c r="Q20" s="40">
         <f>GAME1!G10*2+GAME1!I10*3+GAME1!K10</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="31"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="52"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="3" t="s">
         <v>45</v>
       </c>
@@ -3092,29 +3092,29 @@
       <c r="I21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="39"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="41"/>
     </row>
     <row r="22" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="31">
+      <c r="B22" s="43">
         <f>GAME1!C11</f>
         <v>11</v>
       </c>
-      <c r="C22" s="33" t="str">
+      <c r="C22" s="46" t="str">
         <f>GAME1!D11</f>
         <v>Stevan Džigurski</v>
       </c>
-      <c r="D22" s="50">
+      <c r="D22" s="36">
         <f>GAME1!E11</f>
         <v>15</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="30">
         <f>GAME1!G11*2+GAME1!I11*3+GAME1!K11+GAME1!L11+GAME1!M11+GAME1!N11+GAME1!P11+GAME1!Q11-GAME1!F11-GAME1!H11-GAME1!J11-GAME1!O11</f>
         <v>1</v>
       </c>
@@ -3132,44 +3132,44 @@
       <c r="I22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="31">
+      <c r="J22" s="43">
         <f>GAME1!L11+GAME1!M11</f>
         <v>2</v>
       </c>
-      <c r="K22" s="35">
+      <c r="K22" s="42">
         <f>GAME1!L11</f>
         <v>0</v>
       </c>
-      <c r="L22" s="33">
+      <c r="L22" s="46">
         <f>GAME1!M11</f>
         <v>2</v>
       </c>
-      <c r="M22" s="31">
+      <c r="M22" s="43">
         <f>GAME1!N11</f>
         <v>0</v>
       </c>
-      <c r="N22" s="56">
+      <c r="N22" s="35">
         <f>GAME1!O11</f>
         <v>0</v>
       </c>
-      <c r="O22" s="35">
+      <c r="O22" s="42">
         <f>GAME1!P11</f>
         <v>0</v>
       </c>
-      <c r="P22" s="35">
+      <c r="P22" s="42">
         <f>GAME1!Q11</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="38">
+      <c r="Q22" s="40">
         <f>GAME1!G11*2+GAME1!I11*3+GAME1!K11</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="31"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="3">
         <f>(GAME1!G11+GAME1!I11)/(GAME1!G11+GAME1!F11+GAME1!I11+GAME1!H11)</f>
         <v>0</v>
@@ -3184,29 +3184,29 @@
       <c r="I23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J23" s="31"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="39"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="41"/>
     </row>
     <row r="24" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="31">
+      <c r="B24" s="43">
         <f>GAME1!C12</f>
         <v>12</v>
       </c>
-      <c r="C24" s="33" t="str">
+      <c r="C24" s="46" t="str">
         <f>GAME1!D12</f>
         <v>Marko Vuković</v>
       </c>
-      <c r="D24" s="50">
+      <c r="D24" s="36">
         <f>GAME1!E12</f>
         <v>12</v>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="30">
         <f>GAME1!G12*2+GAME1!I12*3+GAME1!K12+GAME1!L12+GAME1!M12+GAME1!N12+GAME1!P12+GAME1!Q12-GAME1!F12-GAME1!H12-GAME1!J12-GAME1!O12</f>
         <v>0</v>
       </c>
@@ -3225,44 +3225,44 @@
       <c r="I24" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J24" s="31">
+      <c r="J24" s="43">
         <f>GAME1!L12+GAME1!M12</f>
         <v>2</v>
       </c>
-      <c r="K24" s="35">
+      <c r="K24" s="42">
         <f>GAME1!L12</f>
         <v>1</v>
       </c>
-      <c r="L24" s="33">
+      <c r="L24" s="46">
         <f>GAME1!M12</f>
         <v>1</v>
       </c>
-      <c r="M24" s="31">
+      <c r="M24" s="43">
         <f>GAME1!N12</f>
         <v>1</v>
       </c>
-      <c r="N24" s="56">
+      <c r="N24" s="35">
         <f>GAME1!O12</f>
         <v>2</v>
       </c>
-      <c r="O24" s="35">
+      <c r="O24" s="42">
         <f>GAME1!P12</f>
         <v>0</v>
       </c>
-      <c r="P24" s="35">
+      <c r="P24" s="42">
         <f>GAME1!Q12</f>
         <v>0</v>
       </c>
-      <c r="Q24" s="38">
+      <c r="Q24" s="40">
         <f>GAME1!G12*2+GAME1!I12*3+GAME1!K12</f>
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="31"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="52"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="3">
         <f>(GAME1!G12+GAME1!I12)/(GAME1!G12+GAME1!F12+GAME1!I12+GAME1!H12)</f>
         <v>0.25</v>
@@ -3278,29 +3278,29 @@
       <c r="I25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J25" s="31"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="39"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="41"/>
     </row>
     <row r="26" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="31">
+      <c r="B26" s="43">
         <f>GAME1!C13</f>
         <v>13</v>
       </c>
-      <c r="C26" s="33" t="str">
+      <c r="C26" s="46" t="str">
         <f>GAME1!D13</f>
         <v>Bojan Stričević</v>
       </c>
-      <c r="D26" s="50">
+      <c r="D26" s="36">
         <f>GAME1!E13</f>
         <v>30</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="30">
         <f>GAME1!G13*2+GAME1!I13*3+GAME1!K13+GAME1!L13+GAME1!M13+GAME1!N13+GAME1!P13+GAME1!Q13-GAME1!F13-GAME1!H13-GAME1!J13-GAME1!O13</f>
         <v>12</v>
       </c>
@@ -3320,44 +3320,44 @@
         <f>GAME1!K13&amp;"/"&amp;(GAME1!K13+GAME1!J13)</f>
         <v>3/4</v>
       </c>
-      <c r="J26" s="31">
+      <c r="J26" s="43">
         <f>GAME1!L13+GAME1!M13</f>
         <v>6</v>
       </c>
-      <c r="K26" s="35">
+      <c r="K26" s="42">
         <f>GAME1!L13</f>
         <v>1</v>
       </c>
-      <c r="L26" s="33">
+      <c r="L26" s="46">
         <f>GAME1!M13</f>
         <v>5</v>
       </c>
-      <c r="M26" s="31">
+      <c r="M26" s="43">
         <f>GAME1!N13</f>
         <v>1</v>
       </c>
-      <c r="N26" s="56">
+      <c r="N26" s="35">
         <f>GAME1!O13</f>
         <v>2</v>
       </c>
-      <c r="O26" s="35">
+      <c r="O26" s="42">
         <f>GAME1!P13</f>
         <v>1</v>
       </c>
-      <c r="P26" s="35">
+      <c r="P26" s="42">
         <f>GAME1!Q13</f>
         <v>0</v>
       </c>
-      <c r="Q26" s="38">
+      <c r="Q26" s="40">
         <f>GAME1!G13*2+GAME1!I13*3+GAME1!K13</f>
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="31"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="52"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="30"/>
       <c r="F27" s="3">
         <f>(GAME1!G13+GAME1!I13)/(GAME1!G13+GAME1!F13+GAME1!I13+GAME1!H13)</f>
         <v>0.4</v>
@@ -3374,29 +3374,29 @@
         <f>GAME1!K13/(GAME1!K13+GAME1!J13)</f>
         <v>0.75</v>
       </c>
-      <c r="J27" s="31"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="55"/>
-      <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="39"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="41"/>
     </row>
     <row r="28" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="31">
+      <c r="B28" s="43">
         <f>GAME1!C14</f>
         <v>14</v>
       </c>
-      <c r="C28" s="33" t="str">
+      <c r="C28" s="46" t="str">
         <f>GAME1!D14</f>
         <v>Čedomir Erak</v>
       </c>
-      <c r="D28" s="50">
+      <c r="D28" s="36">
         <f>GAME1!E14</f>
         <v>28</v>
       </c>
-      <c r="E28" s="52">
+      <c r="E28" s="30">
         <f>GAME1!G14*2+GAME1!I14*3+GAME1!K14+GAME1!L14+GAME1!M14+GAME1!N14+GAME1!P14+GAME1!Q14-GAME1!F14-GAME1!H14-GAME1!J14-GAME1!O14</f>
         <v>11</v>
       </c>
@@ -3415,44 +3415,44 @@
       <c r="I28" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J28" s="31">
+      <c r="J28" s="43">
         <f>GAME1!L14+GAME1!M14</f>
         <v>8</v>
       </c>
-      <c r="K28" s="35">
+      <c r="K28" s="42">
         <f>GAME1!L14</f>
         <v>2</v>
       </c>
-      <c r="L28" s="33">
+      <c r="L28" s="46">
         <f>GAME1!M14</f>
         <v>6</v>
       </c>
-      <c r="M28" s="31">
+      <c r="M28" s="43">
         <f>GAME1!N14</f>
         <v>1</v>
       </c>
-      <c r="N28" s="56">
+      <c r="N28" s="35">
         <f>GAME1!O14</f>
         <v>0</v>
       </c>
-      <c r="O28" s="35">
+      <c r="O28" s="42">
         <f>GAME1!P14</f>
         <v>0</v>
       </c>
-      <c r="P28" s="35">
+      <c r="P28" s="42">
         <f>GAME1!Q14</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="38">
+      <c r="Q28" s="40">
         <f>GAME1!G14*2+GAME1!I14*3+GAME1!K14</f>
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="31"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="52"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="30"/>
       <c r="F29" s="3">
         <f>(GAME1!G14+GAME1!I14)/(GAME1!G14+GAME1!F14+GAME1!I14+GAME1!H14)</f>
         <v>0.4</v>
@@ -3468,29 +3468,29 @@
       <c r="I29" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J29" s="31"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="39"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="41"/>
     </row>
     <row r="30" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="31">
+      <c r="B30" s="43">
         <f>GAME1!C15</f>
         <v>15</v>
       </c>
-      <c r="C30" s="38" t="str">
+      <c r="C30" s="40" t="str">
         <f>GAME1!D15</f>
         <v>Adrijan Horvat</v>
       </c>
-      <c r="D30" s="50">
+      <c r="D30" s="36">
         <f>GAME1!E15</f>
         <v>30</v>
       </c>
-      <c r="E30" s="52">
+      <c r="E30" s="30">
         <f>GAME1!G15*2+GAME1!I15*3+GAME1!K15+GAME1!L15+GAME1!M15+GAME1!N15+GAME1!P15+GAME1!Q15-GAME1!F15-GAME1!H15-GAME1!J15-GAME1!O15</f>
         <v>15</v>
       </c>
@@ -3510,44 +3510,44 @@
         <f>GAME1!K15&amp;"/"&amp;(GAME1!K15+GAME1!J15)</f>
         <v>4/5</v>
       </c>
-      <c r="J30" s="31">
+      <c r="J30" s="43">
         <f>GAME1!L15+GAME1!M15</f>
         <v>6</v>
       </c>
-      <c r="K30" s="35">
+      <c r="K30" s="42">
         <f>GAME1!L15</f>
         <v>1</v>
       </c>
-      <c r="L30" s="33">
+      <c r="L30" s="46">
         <f>GAME1!M15</f>
         <v>5</v>
       </c>
-      <c r="M30" s="31">
+      <c r="M30" s="43">
         <f>GAME1!N15</f>
         <v>4</v>
       </c>
-      <c r="N30" s="56">
+      <c r="N30" s="35">
         <f>GAME1!O15</f>
         <v>5</v>
       </c>
-      <c r="O30" s="35">
+      <c r="O30" s="42">
         <f>GAME1!P15</f>
         <v>2</v>
       </c>
-      <c r="P30" s="35">
+      <c r="P30" s="42">
         <f>GAME1!Q15</f>
         <v>0</v>
       </c>
-      <c r="Q30" s="38">
+      <c r="Q30" s="40">
         <f>GAME1!G15*2+GAME1!I15*3+GAME1!K15</f>
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:17" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="47"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="50"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="36"/>
       <c r="F31" s="3">
         <f>(GAME1!G15+GAME1!I15)/(GAME1!G15+GAME1!F15+GAME1!I15+GAME1!H15)</f>
         <v>0.5</v>
@@ -3564,25 +3564,25 @@
         <f>GAME1!K15/(GAME1!K15+GAME1!J15)</f>
         <v>0.8</v>
       </c>
-      <c r="J31" s="31"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="55"/>
-      <c r="O31" s="35"/>
-      <c r="P31" s="35"/>
-      <c r="Q31" s="39"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="42"/>
+      <c r="Q31" s="41"/>
     </row>
     <row r="32" spans="2:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="40"/>
-      <c r="C32" s="42" t="s">
+      <c r="B32" s="47"/>
+      <c r="C32" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="53">
+      <c r="D32" s="31">
         <f>SUM(GAME1!E4:'GAME1'!E15)</f>
         <v>207</v>
       </c>
-      <c r="E32" s="57">
+      <c r="E32" s="38">
         <f>SUM(GAME1!G4:'GAME1'!G15)*2+SUM(GAME1!I4:'GAME1'!I15)*3+SUM(GAME1!K4:'GAME1'!K15)+SUM(GAME1!L4:'GAME1'!L15)+SUM(GAME1!M4:'GAME1'!M15)+SUM(GAME1!N4:'GAME1'!N15)+SUM(GAME1!P4:'GAME1'!P15)+SUM(GAME1!Q4:'GAME1'!Q15)-SUM(GAME1!F4:'GAME1'!F15)-SUM(GAME1!H4:'GAME1'!H15)-SUM(GAME1!J4:'GAME1'!J15)-SUM(GAME1!O4:'GAME1'!O15)</f>
         <v>84</v>
       </c>
@@ -3602,44 +3602,44 @@
         <f>SUM(GAME1!K4:'GAME1'!K15)&amp;"/"&amp;(SUM(GAME1!K4:'GAME1'!K15)+SUM(GAME1!J4:'GAME1'!J15))</f>
         <v>13/21</v>
       </c>
-      <c r="J32" s="40">
+      <c r="J32" s="47">
         <f>SUM(GAME1!L4:'GAME1'!L15)+SUM(GAME1!M4:'GAME1'!M15)</f>
         <v>41</v>
       </c>
-      <c r="K32" s="44">
+      <c r="K32" s="33">
         <f>SUM(GAME1!L4:'GAME1'!L15)</f>
         <v>12</v>
       </c>
-      <c r="L32" s="48">
+      <c r="L32" s="53">
         <f>SUM(GAME1!M4:'GAME1'!M15)</f>
         <v>29</v>
       </c>
-      <c r="M32" s="40">
+      <c r="M32" s="47">
         <f>SUM(GAME1!N4:'GAME1'!N15)</f>
         <v>18</v>
       </c>
-      <c r="N32" s="44">
+      <c r="N32" s="33">
         <f>SUM(GAME1!O4:'GAME1'!O15)</f>
         <v>18</v>
       </c>
-      <c r="O32" s="44">
+      <c r="O32" s="33">
         <f>SUM(GAME1!P4:'GAME1'!P15)</f>
         <v>9</v>
       </c>
-      <c r="P32" s="44">
+      <c r="P32" s="33">
         <f>SUM(GAME1!Q4:'GAME1'!Q15)</f>
         <v>6</v>
       </c>
-      <c r="Q32" s="48">
+      <c r="Q32" s="53">
         <f>SUM(GAME1!G4:'GAME1'!G15)*2+SUM(GAME1!I4:'GAME1'!I15)*3+SUM(GAME1!K4:'GAME1'!K15)</f>
         <v>78</v>
       </c>
     </row>
     <row r="33" spans="2:17" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="41"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="58"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="39"/>
       <c r="F33" s="11">
         <f>(SUM(GAME1!G4:'GAME1'!G15)+SUM(GAME1!I4:'GAME1'!I15))/(SUM(GAME1!G4:'GAME1'!G15)+SUM(GAME1!F4:'GAME1'!F15)+SUM(GAME1!I4:'GAME1'!I15)+SUM(GAME1!H4:'GAME1'!H15))</f>
         <v>0.4</v>
@@ -3656,17 +3656,151 @@
         <f>SUM(GAME1!K4:'GAME1'!K15)/(SUM(GAME1!K4:'GAME1'!K15)+SUM(GAME1!J4:'GAME1'!J15))</f>
         <v>0.61904761904761907</v>
       </c>
-      <c r="J33" s="41"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="49"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="51"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="158">
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:Q4"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="Q30:Q31"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="Q32:Q33"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="Q26:Q27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="N30:N31"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="N8:N9"/>
@@ -3691,140 +3825,6 @@
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E26:E27"/>
-    <mergeCell ref="Q28:Q29"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="Q26:Q27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="Q30:Q31"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="P32:P33"/>
-    <mergeCell ref="Q32:Q33"/>
-    <mergeCell ref="N32:N33"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>